<commit_message>
reading file is fixed.
</commit_message>
<xml_diff>
--- a/Source/FaroeIslands.xlsx
+++ b/Source/FaroeIslands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
-    <t>Home</t>
-  </si>
-  <si>
     <t>Home5</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Sandoy, Sku</t>
+  </si>
+  <si>
+    <t>Island</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -438,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1">
         <v>10</v>
@@ -461,10 +461,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -484,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
         <v>10</v>
@@ -507,10 +507,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1">
         <v>10</v>
@@ -530,10 +530,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
         <v>60</v>
@@ -553,10 +553,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>60</v>
@@ -576,10 +576,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1">
         <v>60</v>
@@ -599,10 +599,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
         <v>60</v>
@@ -622,10 +622,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1">
         <v>110</v>

</xml_diff>